<commit_message>
Revised Task Assignments and Iteration plan for E1
</commit_message>
<xml_diff>
--- a/I1/ревизирани файлове 4.12/Team1_Revision/ABM-I1-Task Assignments.xlsx
+++ b/I1/ревизирани файлове 4.12/Team1_Revision/ABM-I1-Task Assignments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSITY\PSS-Rep\PSS\I1\Completed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\PSS\PSS\I1\ревизирани файлове 4.12\Team1_Revision\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -133,9 +133,6 @@
     <t xml:space="preserve">Задачата се предава във формата на създадения документ, приложен в папка "I1/Completed" от общото репозитори. </t>
   </si>
   <si>
-    <t>Създаване на "Списък на рисковете" - подробен списък с рисковете при изпълнението на проекта. Темплейт на документа - "03-Risk-List-tmp.xls". Също така, да се създаде и да се разпишат всички точки от документа "План за управление на рисковете и проблемите". Темплейт - "02-Risk-Management-Plan-rup_rskpln.dot". Време за изпълнение: 12 часа</t>
-  </si>
-  <si>
     <t xml:space="preserve">Задачата се предава във формата на създадените документи, приложени в папка "I1/Completed" от общото репозитори. </t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>Калоян</t>
   </si>
   <si>
-    <t xml:space="preserve">Създаване на документа "Спецификация на допълнителните изисквания" (SRS). Да се разпишат подробно функционалностите на разработваната система. Да се групират и обособят, като се изведат модулите на системата. Да се попълнят и подробно разпишат всички точки на споменатия документ. Темплейт - "02-Requirements-Management-Plan-rup_rmpln.dot". Време за изпълнение: 8 часа. </t>
-  </si>
-  <si>
     <t>Задачата се предава във формата на създадения документ, приложен в папка "I1/Completed" от общото репозитори. Заедно с документа да се предаде и друг документ, който съдържа описание на изведените модули на системата и списък с функционалностите им</t>
   </si>
   <si>
@@ -163,34 +157,40 @@
     <t>Борислав и Мартин</t>
   </si>
   <si>
-    <t>Създаване на "План за изпълнение на итерация E1 от общия план". Да се създаде документ подобен на текущия (или ако имаме възможност в Jira), който да дава подробна информация относно изпълнението на следващата итерация от проекта - Е1. Да се разпишат и възложат необходимите задачи, като се определи време за изпълнение и се запише подробно описание на типа на задачата и начина, по който да бъдат представени резултатите. Определено време за изпълнение - 6 часа</t>
-  </si>
-  <si>
-    <t>Създаване на документа "План за разработка на софтуерния продукт". Темплейт - "01-rup_sdpln.dot". Подробно разписване и попълване на всички точки от документа. Определено време за изпълнение - около 12 часа.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Създаване на документа "Речник". Темплейт - "rup_gloss.dot". Подробно описание на всички точки на документа. След създаването му, документът е подготвен и отворен към всички участници в разработката, които имат необходимостта да го ползват/допълват. </t>
-  </si>
-  <si>
-    <t>Създаване на документ "График за изпълнението на проекта". Темплейт - "07-0-1-Example-Project-Schedule.mpp".  Да се създаде подробен график по изпълнението, като се разпишат фазите, итерациите и задачите, както и сроковете за изпълнение. Време за изпълнение: 16 часа</t>
-  </si>
-  <si>
     <t>Борислав и Калоян</t>
   </si>
   <si>
-    <t>Създаване на "План за управление на качеството". Темплейт - "02-Quality-Assurance-Plan-rup_qapln". Подробно разписване и попълване на всички точки от документа. Определено време за изпълнение - около 12 часа</t>
-  </si>
-  <si>
-    <t>Създаване на документа "Конвенции за писане на код". Темплейт - "rup_prggd.dot". Подробно разписване и попълване на всички точки от документа. Определено време за изпълнение - около 4 часа.</t>
-  </si>
-  <si>
     <t>ABM-0</t>
+  </si>
+  <si>
+    <t>Създаване на "Списък на рисковете" - подробен списък с рисковете при изпълнението на проекта. Темплейт на документа - "03-Risk-List-tmp.xls". Също така, да се създаде и да се разпишат всички точки от документа "План за управление на рисковете и проблемите". Темплейт - "02-Risk-Management-Plan-rup_rskpln.dot". Време за изпълнение: 3 дни</t>
+  </si>
+  <si>
+    <t>Създаване на документа "Речник". Темплейт - "rup_gloss.dot". Подробно описание на всички точки на документа. След създаването му, документът е подготвен и отворен към всички участници в разработката, които имат необходимостта да го ползват/допълват. - 2 дни</t>
+  </si>
+  <si>
+    <t>Създаване на документ "График за изпълнението на проекта". Темплейт - "07-0-1-Example-Project-Schedule.mpp".  Да се създаде подробен график по изпълнението, като се разпишат фазите, итерациите и задачите, както и сроковете за изпълнение. Време за изпълнение: 4 дни</t>
+  </si>
+  <si>
+    <t>Създаване на документа "Спецификация на допълнителните изисквания" (SRS). Да се разпишат подробно функционалностите на разработваната система. Да се групират и обособят, като се изведат модулите на системата. Да се попълнят и подробно разпишат всички точки на споменатия документ. Темплейт - "02-Requirements-Management-Plan-rup_rmpln.dot". Време за изпълнение: 2 дни</t>
+  </si>
+  <si>
+    <t>Създаване на "План за изпълнение на итерация E1 от общия план". Да се създаде документ подобен на текущия (или ако имаме възможност в Jira), който да дава подробна информация относно изпълнението на следващата итерация от проекта - Е1. Да се разпишат и възложат необходимите задачи, като се определи време за изпълнение и се запише подробно описание на типа на задачата и начина, по който да бъдат представени резултатите. Определено време за изпълнение - 3 дни</t>
+  </si>
+  <si>
+    <t>Създаване на документа "Конвенции за писане на код". Темплейт - "rup_prggd.dot". Подробно разписване и попълване на всички точки от документа. Определено време за изпълнение - около 3 дни</t>
+  </si>
+  <si>
+    <t>Създаване на "План за управление на качеството". Темплейт - "02-Quality-Assurance-Plan-rup_qapln". Подробно разписване и попълване на всички точки от документа. Определено време за изпълнение - около 4 дни</t>
+  </si>
+  <si>
+    <t>Създаване на документа "План за разработка на софтуерния продукт". Темплейт - "01-rup_sdpln.dot". Подробно разписване и попълване на всички точки от документа. Определено време за изпълнение - около 4 дни</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -676,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C2" s="13">
         <v>42338</v>
@@ -694,7 +694,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I2" s="13">
         <v>42311</v>
@@ -726,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="I3" s="13">
         <v>42311</v>
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>30</v>
@@ -758,7 +758,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I4" s="13">
         <v>42311</v>
@@ -790,13 +790,13 @@
         <v>22</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="I5" s="13">
         <v>42311</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="63.75" collapsed="1" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="13">
         <v>42338</v>
@@ -822,7 +822,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" s="13">
         <v>42309</v>
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="13">
         <v>42338</v>
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>30</v>
@@ -854,13 +854,13 @@
         <v>22</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I7" s="13">
         <v>42311</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="38.25" collapsed="1" x14ac:dyDescent="0.2">
@@ -868,7 +868,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="13">
         <v>42338</v>
@@ -886,7 +886,7 @@
         <v>23</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="13">
         <v>42311</v>
@@ -900,7 +900,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="13">
         <v>42338</v>
@@ -909,7 +909,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>30</v>
@@ -918,7 +918,7 @@
         <v>22</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" s="13">
         <v>42311</v>

</xml_diff>